<commit_message>
Update table 2 and 3
</commit_message>
<xml_diff>
--- a/tables/03_output/table2_2020_2021.xlsx
+++ b/tables/03_output/table2_2020_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braul\Desktop\05_personal_projects\Vol07_InnovaLab\01_excess_mortality\db_SINADEF\5. Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braul\Desktop\05_personal_projects\01_GITHUB\Excess_Mort\tables\03_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B8706B-356D-4B2F-969B-B54BC95D0931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042FE386-9D98-4979-8EDB-3BC3ABE8020E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8568" yWindow="7404" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4740" yWindow="5052" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,19 +124,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -440,9 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -453,25 +448,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="5">
         <v>2020</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -484,11 +479,11 @@
         <v>22125</v>
       </c>
       <c r="E3" s="1">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -499,11 +494,11 @@
         <v>43655</v>
       </c>
       <c r="E4" s="1">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -514,11 +509,11 @@
         <v>93773</v>
       </c>
       <c r="E5" s="1">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -529,11 +524,11 @@
         <v>66252</v>
       </c>
       <c r="E6" s="1">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -543,12 +538,12 @@
       <c r="D7" s="2">
         <v>225805</v>
       </c>
-      <c r="E7" s="2">
-        <v>1.8</v>
+      <c r="E7" s="7">
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="5">
         <v>2021</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -561,11 +556,11 @@
         <v>25684</v>
       </c>
       <c r="E8" s="1">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="5">
         <v>2021</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -578,11 +573,11 @@
         <v>52698</v>
       </c>
       <c r="E9" s="1">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="5">
         <v>2021</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -595,11 +590,11 @@
         <v>100565</v>
       </c>
       <c r="E10" s="1">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="5">
         <v>2021</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -612,11 +607,11 @@
         <v>67984</v>
       </c>
       <c r="E11" s="1">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="6">
         <v>2021</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -629,7 +624,7 @@
         <v>246931</v>
       </c>
       <c r="E12" s="7">
-        <v>2</v>
+        <v>0.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>